<commit_message>
Change institution name to english in db seed
</commit_message>
<xml_diff>
--- a/fixtures/recommender-test.xlsx
+++ b/fixtures/recommender-test.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wells/project/qs-survey/fixtures/recommenders_upload/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wells/project/qs-survey/fixtures/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F7A76F8-16A4-9C4C-BAFA-FF2A3508328D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9D6825D-4F0C-C240-8137-AD4A7A584E5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28800" yWindow="11060" windowWidth="38400" windowHeight="10540" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28800" yWindow="500" windowWidth="38400" windowHeight="21100" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="填寫說明" sheetId="1" r:id="rId1"/>
@@ -1327,10 +1327,6 @@
     <t>ymhsieh@mail.ntust.edu.tw</t>
   </si>
   <si>
-    <t>臺灣科技大學</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>Department of Civil and Construction Engineering</t>
   </si>
   <si>
@@ -1355,6 +1351,9 @@
   <si>
     <t>adv</t>
     <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>National Taiwan University of Science and Technology</t>
   </si>
 </sst>
 </file>
@@ -2134,6 +2133,15 @@
     <xf numFmtId="49" fontId="19" fillId="34" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="36" fillId="0" borderId="0" xfId="42" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="36" fillId="0" borderId="0" xfId="42" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -2142,15 +2150,6 @@
     </xf>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="36" fillId="0" borderId="0" xfId="42" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="36" fillId="0" borderId="0" xfId="42" applyNumberFormat="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="43">
@@ -2491,32 +2490,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="18.75" customHeight="1">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
-      <c r="F1" s="14"/>
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
     </row>
     <row r="2" spans="1:6" s="2" customFormat="1" ht="409.5" customHeight="1">
-      <c r="A2" s="15" t="s">
+      <c r="A2" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="15"/>
-      <c r="C2" s="15"/>
-      <c r="D2" s="15"/>
-      <c r="E2" s="15"/>
-      <c r="F2" s="15"/>
+      <c r="B2" s="18"/>
+      <c r="C2" s="18"/>
+      <c r="D2" s="18"/>
+      <c r="E2" s="18"/>
+      <c r="F2" s="18"/>
     </row>
     <row r="9" spans="1:6" ht="32.25" customHeight="1">
-      <c r="A9" s="13"/>
-      <c r="B9" s="13"/>
-      <c r="C9" s="13"/>
-      <c r="D9" s="13"/>
-      <c r="E9" s="13"/>
-      <c r="F9" s="13"/>
+      <c r="A9" s="16"/>
+      <c r="B9" s="16"/>
+      <c r="C9" s="16"/>
+      <c r="D9" s="16"/>
+      <c r="E9" s="16"/>
+      <c r="F9" s="16"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -2538,7 +2537,7 @@
   <dimension ref="A1:J16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="H30" sqref="H30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.6640625" defaultRowHeight="16"/>
@@ -2589,13 +2588,13 @@
       <c r="I2" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="J2" s="18"/>
+      <c r="J2" s="15"/>
     </row>
     <row r="3" spans="1:10">
       <c r="A3" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="B3" s="16" t="s">
+      <c r="B3" s="13" t="s">
         <v>78</v>
       </c>
       <c r="C3" s="4" t="s">
@@ -2611,10 +2610,10 @@
         <v>82</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>84</v>
+        <v>91</v>
       </c>
       <c r="I3" s="4" t="s">
         <v>83</v>
@@ -2624,7 +2623,7 @@
       <c r="A4" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="B4" s="16" t="s">
+      <c r="B4" s="13" t="s">
         <v>78</v>
       </c>
       <c r="C4" s="4" t="s">
@@ -2637,13 +2636,13 @@
         <v>82</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>84</v>
+        <v>91</v>
       </c>
       <c r="I4" s="4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="16" spans="1:10">
@@ -2726,7 +2725,7 @@
       <c r="A3" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="B3" s="16" t="s">
+      <c r="B3" s="13" t="s">
         <v>78</v>
       </c>
       <c r="C3" s="4" t="s">
@@ -2739,16 +2738,16 @@
         <v>81</v>
       </c>
       <c r="F3" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="G3" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="G3" s="4" t="s">
+      <c r="H3" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="H3" s="4" t="s">
+      <c r="I3" s="4" t="s">
         <v>88</v>
-      </c>
-      <c r="I3" s="4" t="s">
-        <v>89</v>
       </c>
       <c r="J3" s="4" t="s">
         <v>83</v>
@@ -2758,26 +2757,26 @@
       <c r="A4" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="B4" s="16" t="s">
+      <c r="B4" s="13" t="s">
         <v>78</v>
       </c>
       <c r="D4" s="4" t="s">
         <v>80</v>
       </c>
       <c r="F4" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="G4" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="G4" s="4" t="s">
+      <c r="H4" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="H4" s="4" t="s">
+      <c r="I4" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="I4" s="4" t="s">
+      <c r="J4" s="14" t="s">
         <v>89</v>
-      </c>
-      <c r="J4" s="17" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="16" spans="1:10">

</xml_diff>

<commit_message>
fix: test error after use InstitutionInput
</commit_message>
<xml_diff>
--- a/fixtures/recommender-test.xlsx
+++ b/fixtures/recommender-test.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10611"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10911"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wells/project/qs-survey/fixtures/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9D6825D-4F0C-C240-8137-AD4A7A584E5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45D76DB6-7A3F-3C49-979D-FB36C8A1A01A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28800" yWindow="500" windowWidth="38400" windowHeight="21100" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="填寫說明" sheetId="1" r:id="rId1"/>
@@ -1341,10 +1341,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>Taiwan, Province of China</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>212f2f@gmail.com</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -1354,6 +1350,10 @@
   </si>
   <si>
     <t>National Taiwan University of Science and Technology</t>
+  </si>
+  <si>
+    <t>Taiwan</t>
+    <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -2093,14 +2093,11 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="24" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
@@ -2139,7 +2136,7 @@
     <xf numFmtId="49" fontId="36" fillId="0" borderId="0" xfId="42" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -2490,32 +2487,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="18.75" customHeight="1">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="17"/>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
-      <c r="E1" s="17"/>
-      <c r="F1" s="17"/>
-    </row>
-    <row r="2" spans="1:6" s="2" customFormat="1" ht="409.5" customHeight="1">
-      <c r="A2" s="18" t="s">
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
+    </row>
+    <row r="2" spans="1:6" ht="409.5" customHeight="1">
+      <c r="A2" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="18"/>
-      <c r="C2" s="18"/>
-      <c r="D2" s="18"/>
-      <c r="E2" s="18"/>
-      <c r="F2" s="18"/>
+      <c r="B2" s="17"/>
+      <c r="C2" s="17"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="17"/>
+      <c r="F2" s="17"/>
     </row>
     <row r="9" spans="1:6" ht="32.25" customHeight="1">
-      <c r="A9" s="16"/>
-      <c r="B9" s="16"/>
-      <c r="C9" s="16"/>
-      <c r="D9" s="16"/>
-      <c r="E9" s="16"/>
-      <c r="F9" s="16"/>
+      <c r="A9" s="15"/>
+      <c r="B9" s="15"/>
+      <c r="C9" s="15"/>
+      <c r="D9" s="15"/>
+      <c r="E9" s="15"/>
+      <c r="F9" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -2536,117 +2533,117 @@
   </sheetPr>
   <dimension ref="A1:J16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H30" sqref="H30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.6640625" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="11.33203125" style="4" customWidth="1"/>
-    <col min="2" max="2" width="15.83203125" style="4" customWidth="1"/>
-    <col min="3" max="3" width="9.6640625" style="4"/>
-    <col min="4" max="4" width="11.33203125" style="4" customWidth="1"/>
-    <col min="5" max="5" width="11.6640625" style="4" customWidth="1"/>
-    <col min="6" max="6" width="17" style="4" customWidth="1"/>
-    <col min="7" max="7" width="18.6640625" style="4" customWidth="1"/>
-    <col min="8" max="8" width="30.1640625" style="4" customWidth="1"/>
-    <col min="9" max="9" width="24.83203125" style="4" customWidth="1"/>
-    <col min="10" max="10" width="31.1640625" style="4" customWidth="1"/>
-    <col min="11" max="16384" width="9.6640625" style="4"/>
+    <col min="1" max="1" width="11.33203125" style="3" customWidth="1"/>
+    <col min="2" max="2" width="15.83203125" style="3" customWidth="1"/>
+    <col min="3" max="3" width="9.6640625" style="3"/>
+    <col min="4" max="4" width="11.33203125" style="3" customWidth="1"/>
+    <col min="5" max="5" width="11.6640625" style="3" customWidth="1"/>
+    <col min="6" max="6" width="17" style="3" customWidth="1"/>
+    <col min="7" max="7" width="18.6640625" style="3" customWidth="1"/>
+    <col min="8" max="8" width="30.1640625" style="3" customWidth="1"/>
+    <col min="9" max="9" width="24.83203125" style="3" customWidth="1"/>
+    <col min="10" max="10" width="31.1640625" style="3" customWidth="1"/>
+    <col min="11" max="16384" width="9.6640625" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="23.25" customHeight="1">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="4" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="33.75" customHeight="1">
-      <c r="A2" s="12" t="s">
+      <c r="A2" s="11" t="s">
         <v>75</v>
       </c>
-      <c r="B2" s="11" t="s">
+      <c r="B2" s="10" t="s">
         <v>76</v>
       </c>
-      <c r="C2" s="9" t="s">
+      <c r="C2" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="9" t="s">
+      <c r="D2" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="9" t="s">
+      <c r="E2" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="9" t="s">
+      <c r="F2" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="G2" s="9" t="s">
+      <c r="G2" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="H2" s="9" t="s">
+      <c r="H2" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="I2" s="9" t="s">
+      <c r="I2" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="J2" s="15"/>
+      <c r="J2" s="14"/>
     </row>
     <row r="3" spans="1:10">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="B3" s="13" t="s">
+      <c r="B3" s="12" t="s">
         <v>78</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D3" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="E3" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="F3" s="4" t="s">
+      <c r="F3" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="G3" s="4" t="s">
+      <c r="G3" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="H3" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="I3" s="4" t="s">
+      <c r="H3" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="I3" s="3" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="4" spans="1:10">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="B4" s="13" t="s">
+      <c r="B4" s="12" t="s">
         <v>78</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="E4" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="F4" s="4" t="s">
+      <c r="F4" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="G4" s="4" t="s">
+      <c r="G4" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="H4" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="I4" s="4" t="s">
+      <c r="H4" s="3" t="s">
         <v>90</v>
       </c>
+      <c r="I4" s="3" t="s">
+        <v>89</v>
+      </c>
     </row>
     <row r="16" spans="1:10">
-      <c r="J16" s="3"/>
+      <c r="J16" s="2"/>
     </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
@@ -2665,122 +2662,122 @@
   </sheetPr>
   <dimension ref="A1:J16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.6640625" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="11.83203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.6640625" style="4"/>
-    <col min="4" max="4" width="11.33203125" style="4" customWidth="1"/>
-    <col min="5" max="5" width="11.6640625" style="4" customWidth="1"/>
-    <col min="6" max="6" width="17" style="4" customWidth="1"/>
-    <col min="7" max="7" width="29.6640625" style="4" customWidth="1"/>
-    <col min="8" max="8" width="30.1640625" style="4" customWidth="1"/>
-    <col min="9" max="9" width="13.83203125" style="4" customWidth="1"/>
-    <col min="10" max="10" width="31.1640625" style="4" customWidth="1"/>
-    <col min="11" max="16384" width="9.6640625" style="4"/>
+    <col min="1" max="1" width="11.83203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.6640625" style="3"/>
+    <col min="4" max="4" width="11.33203125" style="3" customWidth="1"/>
+    <col min="5" max="5" width="11.6640625" style="3" customWidth="1"/>
+    <col min="6" max="6" width="17" style="3" customWidth="1"/>
+    <col min="7" max="7" width="29.6640625" style="3" customWidth="1"/>
+    <col min="8" max="8" width="30.1640625" style="3" customWidth="1"/>
+    <col min="9" max="9" width="13.83203125" style="3" customWidth="1"/>
+    <col min="10" max="10" width="31.1640625" style="3" customWidth="1"/>
+    <col min="11" max="16384" width="9.6640625" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="24" customHeight="1">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="4" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="33.75" customHeight="1">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="C2" s="10" t="s">
+      <c r="C2" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="D2" s="10" t="s">
+      <c r="D2" s="9" t="s">
         <v>69</v>
       </c>
-      <c r="E2" s="10" t="s">
+      <c r="E2" s="9" t="s">
         <v>70</v>
       </c>
-      <c r="F2" s="10" t="s">
+      <c r="F2" s="9" t="s">
         <v>64</v>
       </c>
-      <c r="G2" s="10" t="s">
+      <c r="G2" s="9" t="s">
         <v>74</v>
       </c>
-      <c r="H2" s="10" t="s">
+      <c r="H2" s="9" t="s">
         <v>71</v>
       </c>
-      <c r="I2" s="10" t="s">
+      <c r="I2" s="9" t="s">
         <v>72</v>
       </c>
-      <c r="J2" s="10" t="s">
+      <c r="J2" s="9" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="3" spans="1:10">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="B3" s="13" t="s">
+      <c r="B3" s="12" t="s">
         <v>78</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D3" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="E3" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="F3" s="4" t="s">
+      <c r="F3" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="G3" s="4" t="s">
+      <c r="G3" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="H3" s="4" t="s">
+      <c r="H3" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="I3" s="4" t="s">
+      <c r="I3" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
+      <c r="A4" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="B4" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="J4" s="13" t="s">
         <v>88</v>
       </c>
-      <c r="J3" s="4" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10">
-      <c r="A4" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="B4" s="13" t="s">
-        <v>78</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="F4" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="G4" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="H4" s="4" t="s">
-        <v>87</v>
-      </c>
-      <c r="I4" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="J4" s="14" t="s">
-        <v>89</v>
-      </c>
     </row>
     <row r="16" spans="1:10">
-      <c r="J16" s="3"/>
+      <c r="J16" s="2"/>
     </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
@@ -2819,292 +2816,292 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1" ht="18">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="5" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:1" ht="16">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="6" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="16">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="6" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:1" ht="16">
-      <c r="A4" s="7" t="s">
+      <c r="A4" s="6" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:1" ht="16">
-      <c r="A5" s="7" t="s">
+      <c r="A5" s="6" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:1" ht="16">
-      <c r="A6" s="7" t="s">
+      <c r="A6" s="6" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:1" ht="16">
-      <c r="A7" s="7" t="s">
+      <c r="A7" s="6" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="8" spans="1:1" ht="16">
-      <c r="A8" s="7" t="s">
+      <c r="A8" s="6" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="9" spans="1:1" ht="16">
-      <c r="A9" s="7" t="s">
+      <c r="A9" s="6" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="10" spans="1:1" ht="16">
-      <c r="A10" s="7" t="s">
+      <c r="A10" s="6" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="11" spans="1:1" ht="16">
-      <c r="A11" s="7" t="s">
+      <c r="A11" s="6" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="12" spans="1:1" ht="16">
-      <c r="A12" s="7" t="s">
+      <c r="A12" s="6" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="13" spans="1:1" ht="16">
-      <c r="A13" s="7" t="s">
+      <c r="A13" s="6" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="14" spans="1:1" ht="16">
-      <c r="A14" s="7" t="s">
+      <c r="A14" s="6" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="15" spans="1:1" ht="16">
-      <c r="A15" s="7" t="s">
+      <c r="A15" s="6" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="16" spans="1:1" ht="16">
-      <c r="A16" s="7" t="s">
+      <c r="A16" s="6" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="17" spans="1:1" ht="16">
-      <c r="A17" s="7" t="s">
+      <c r="A17" s="6" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="18" spans="1:1" ht="16">
-      <c r="A18" s="7" t="s">
+      <c r="A18" s="6" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="19" spans="1:1" ht="16">
-      <c r="A19" s="7" t="s">
+      <c r="A19" s="6" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="20" spans="1:1" ht="16">
-      <c r="A20" s="7" t="s">
+      <c r="A20" s="6" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="21" spans="1:1" ht="16">
-      <c r="A21" s="7" t="s">
+      <c r="A21" s="6" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="22" spans="1:1" ht="16">
-      <c r="A22" s="7" t="s">
+      <c r="A22" s="6" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="23" spans="1:1" ht="16">
-      <c r="A23" s="7" t="s">
+      <c r="A23" s="6" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="24" spans="1:1" ht="16">
-      <c r="A24" s="7" t="s">
+      <c r="A24" s="6" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="25" spans="1:1" ht="16">
-      <c r="A25" s="7" t="s">
+      <c r="A25" s="6" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="26" spans="1:1" ht="16">
-      <c r="A26" s="7" t="s">
+      <c r="A26" s="6" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="27" spans="1:1" ht="16">
-      <c r="A27" s="7" t="s">
+      <c r="A27" s="6" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="28" spans="1:1" ht="16">
-      <c r="A28" s="7" t="s">
+      <c r="A28" s="6" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="29" spans="1:1" ht="16">
-      <c r="A29" s="7" t="s">
+      <c r="A29" s="6" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="30" spans="1:1" ht="16">
-      <c r="A30" s="7" t="s">
+      <c r="A30" s="6" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="31" spans="1:1" ht="16">
-      <c r="A31" s="7" t="s">
+      <c r="A31" s="6" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="32" spans="1:1" ht="16">
-      <c r="A32" s="7" t="s">
+      <c r="A32" s="6" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="33" spans="1:1" ht="16">
-      <c r="A33" s="7" t="s">
+      <c r="A33" s="6" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="34" spans="1:1" ht="16">
-      <c r="A34" s="7" t="s">
+      <c r="A34" s="6" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="35" spans="1:1" ht="16">
-      <c r="A35" s="7" t="s">
+      <c r="A35" s="6" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="36" spans="1:1" ht="16">
-      <c r="A36" s="7" t="s">
+      <c r="A36" s="6" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="37" spans="1:1" ht="16">
-      <c r="A37" s="7" t="s">
+      <c r="A37" s="6" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="38" spans="1:1" ht="16">
-      <c r="A38" s="7" t="s">
+      <c r="A38" s="6" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="39" spans="1:1" ht="16">
-      <c r="A39" s="7" t="s">
+      <c r="A39" s="6" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="40" spans="1:1" ht="16">
-      <c r="A40" s="7" t="s">
+      <c r="A40" s="6" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="41" spans="1:1" ht="16">
-      <c r="A41" s="7" t="s">
+      <c r="A41" s="6" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="42" spans="1:1" ht="16">
-      <c r="A42" s="7" t="s">
+      <c r="A42" s="6" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="43" spans="1:1" ht="16">
-      <c r="A43" s="7" t="s">
+      <c r="A43" s="6" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="44" spans="1:1" ht="16">
-      <c r="A44" s="7" t="s">
+      <c r="A44" s="6" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="45" spans="1:1" ht="16">
-      <c r="A45" s="7" t="s">
+      <c r="A45" s="6" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="46" spans="1:1" ht="16">
-      <c r="A46" s="7" t="s">
+      <c r="A46" s="6" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="47" spans="1:1" ht="16">
-      <c r="A47" s="7" t="s">
+      <c r="A47" s="6" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="48" spans="1:1" ht="16">
-      <c r="A48" s="7" t="s">
+      <c r="A48" s="6" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="49" spans="1:1" ht="16">
-      <c r="A49" s="7" t="s">
+      <c r="A49" s="6" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="50" spans="1:1" ht="16">
-      <c r="A50" s="7" t="s">
+      <c r="A50" s="6" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="51" spans="1:1" ht="16">
-      <c r="A51" s="7" t="s">
+      <c r="A51" s="6" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="52" spans="1:1" ht="16">
-      <c r="A52" s="7" t="s">
+      <c r="A52" s="6" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="53" spans="1:1" ht="16">
-      <c r="A53" s="7" t="s">
+      <c r="A53" s="6" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="54" spans="1:1" ht="16">
-      <c r="A54" s="7" t="s">
+      <c r="A54" s="6" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="55" spans="1:1" ht="16">
-      <c r="A55" s="7" t="s">
+      <c r="A55" s="6" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="56" spans="1:1" ht="16">
-      <c r="A56" s="7" t="s">
+      <c r="A56" s="6" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="57" spans="1:1" ht="16">
-      <c r="A57" s="7" t="s">
+      <c r="A57" s="6" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="58" spans="1:1" ht="16">
-      <c r="A58" s="7"/>
+      <c r="A58" s="6"/>
     </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>

</xml_diff>

<commit_message>
feat: Add location to excel template
</commit_message>
<xml_diff>
--- a/fixtures/recommender-test.xlsx
+++ b/fixtures/recommender-test.xlsx
@@ -8,22 +8,23 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wells/project/qs-survey/fixtures/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45D76DB6-7A3F-3C49-979D-FB36C8A1A01A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71EDE458-299B-DC4B-BC99-541602520CD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="填寫說明" sheetId="1" r:id="rId1"/>
     <sheet name="聲譽調查提名名冊-學界" sheetId="2" r:id="rId2"/>
     <sheet name="聲譽調查提名名冊-業界" sheetId="4" r:id="rId3"/>
-    <sheet name="工作表3" sheetId="5" state="hidden" r:id="rId4"/>
+    <sheet name="工作表1" sheetId="6" state="hidden" r:id="rId4"/>
+    <sheet name="工作表3" sheetId="5" state="hidden" r:id="rId5"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="370" uniqueCount="344">
   <si>
     <r>
       <t xml:space="preserve">Title
@@ -1300,6 +1301,781 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
+    <t>Afghanistan</t>
+  </si>
+  <si>
+    <t>Aland Islands</t>
+  </si>
+  <si>
+    <t>Albania</t>
+  </si>
+  <si>
+    <t>Algeria</t>
+  </si>
+  <si>
+    <t>American Samoa</t>
+  </si>
+  <si>
+    <t>Andorra</t>
+  </si>
+  <si>
+    <t>Angola</t>
+  </si>
+  <si>
+    <t>Anguilla</t>
+  </si>
+  <si>
+    <t>Antarctica</t>
+  </si>
+  <si>
+    <t>Antigua and Barbuda</t>
+  </si>
+  <si>
+    <t>Argentina</t>
+  </si>
+  <si>
+    <t>Armenia</t>
+  </si>
+  <si>
+    <t>Aruba</t>
+  </si>
+  <si>
+    <t>Australia</t>
+  </si>
+  <si>
+    <t>Austria</t>
+  </si>
+  <si>
+    <t>Azerbaijan</t>
+  </si>
+  <si>
+    <t>Bahamas</t>
+  </si>
+  <si>
+    <t>Bahrain</t>
+  </si>
+  <si>
+    <t>Bangladesh</t>
+  </si>
+  <si>
+    <t>Barbados</t>
+  </si>
+  <si>
+    <t>Belarus</t>
+  </si>
+  <si>
+    <t>Belgium</t>
+  </si>
+  <si>
+    <t>Belize</t>
+  </si>
+  <si>
+    <t>Benin</t>
+  </si>
+  <si>
+    <t>Bermuda</t>
+  </si>
+  <si>
+    <t>Bhutan</t>
+  </si>
+  <si>
+    <t>Bolivia</t>
+  </si>
+  <si>
+    <t>Bonaire, Sint Eustatius and Saba</t>
+  </si>
+  <si>
+    <t>Bosnia and Herzegovina</t>
+  </si>
+  <si>
+    <t>Botswana</t>
+  </si>
+  <si>
+    <t>Bouvet Island</t>
+  </si>
+  <si>
+    <t>Brazil</t>
+  </si>
+  <si>
+    <t>British Indian Ocean Territory</t>
+  </si>
+  <si>
+    <t>Brunei Darussalam</t>
+  </si>
+  <si>
+    <t>Bulgaria</t>
+  </si>
+  <si>
+    <t>Burkina Faso</t>
+  </si>
+  <si>
+    <t>Burundi</t>
+  </si>
+  <si>
+    <t>Cambodia</t>
+  </si>
+  <si>
+    <t>Cameroon</t>
+  </si>
+  <si>
+    <t>Canada</t>
+  </si>
+  <si>
+    <t>Cape Verde</t>
+  </si>
+  <si>
+    <t>Cayman Islands</t>
+  </si>
+  <si>
+    <t>Central African Republic</t>
+  </si>
+  <si>
+    <t>Chad</t>
+  </si>
+  <si>
+    <t>Chile</t>
+  </si>
+  <si>
+    <t>China</t>
+  </si>
+  <si>
+    <t>Christmas Island</t>
+  </si>
+  <si>
+    <t>Cocos (Keeling) Islands</t>
+  </si>
+  <si>
+    <t>Colombia</t>
+  </si>
+  <si>
+    <t>Comoros</t>
+  </si>
+  <si>
+    <t>Congo</t>
+  </si>
+  <si>
+    <t>Congo, Democratic Republic of the Congo</t>
+  </si>
+  <si>
+    <t>Cook Islands</t>
+  </si>
+  <si>
+    <t>Costa Rica</t>
+  </si>
+  <si>
+    <t>Cote D'Ivoire</t>
+  </si>
+  <si>
+    <t>Croatia</t>
+  </si>
+  <si>
+    <t>Cuba</t>
+  </si>
+  <si>
+    <t>Curacao</t>
+  </si>
+  <si>
+    <t>Cyprus</t>
+  </si>
+  <si>
+    <t>Czech Republic</t>
+  </si>
+  <si>
+    <t>Denmark</t>
+  </si>
+  <si>
+    <t>Djibouti</t>
+  </si>
+  <si>
+    <t>Dominica</t>
+  </si>
+  <si>
+    <t>Dominican Republic</t>
+  </si>
+  <si>
+    <t>Ecuador</t>
+  </si>
+  <si>
+    <t>Egypt</t>
+  </si>
+  <si>
+    <t>El Salvador</t>
+  </si>
+  <si>
+    <t>Equatorial Guinea</t>
+  </si>
+  <si>
+    <t>Eritrea</t>
+  </si>
+  <si>
+    <t>Estonia</t>
+  </si>
+  <si>
+    <t>Ethiopia</t>
+  </si>
+  <si>
+    <t>Falkland Islands (Malvinas)</t>
+  </si>
+  <si>
+    <t>Faroe Islands</t>
+  </si>
+  <si>
+    <t>Fiji</t>
+  </si>
+  <si>
+    <t>Finland</t>
+  </si>
+  <si>
+    <t>France</t>
+  </si>
+  <si>
+    <t>French Guiana</t>
+  </si>
+  <si>
+    <t>French Polynesia</t>
+  </si>
+  <si>
+    <t>French Southern Territories</t>
+  </si>
+  <si>
+    <t>Gabon</t>
+  </si>
+  <si>
+    <t>Gambia</t>
+  </si>
+  <si>
+    <t>Georgia</t>
+  </si>
+  <si>
+    <t>Germany</t>
+  </si>
+  <si>
+    <t>Ghana</t>
+  </si>
+  <si>
+    <t>Gibraltar</t>
+  </si>
+  <si>
+    <t>Greece</t>
+  </si>
+  <si>
+    <t>Greenland</t>
+  </si>
+  <si>
+    <t>Grenada</t>
+  </si>
+  <si>
+    <t>Guadeloupe</t>
+  </si>
+  <si>
+    <t>Guam</t>
+  </si>
+  <si>
+    <t>Guatemala</t>
+  </si>
+  <si>
+    <t>Guernsey</t>
+  </si>
+  <si>
+    <t>Guinea</t>
+  </si>
+  <si>
+    <t>Guinea-Bissau</t>
+  </si>
+  <si>
+    <t>Guyana</t>
+  </si>
+  <si>
+    <t>Haiti</t>
+  </si>
+  <si>
+    <t>Heard Island and Mcdonald Islands</t>
+  </si>
+  <si>
+    <t>Holy See (Vatican City State)</t>
+  </si>
+  <si>
+    <t>Honduras</t>
+  </si>
+  <si>
+    <t>Hong Kong</t>
+  </si>
+  <si>
+    <t>Hungary</t>
+  </si>
+  <si>
+    <t>Iceland</t>
+  </si>
+  <si>
+    <t>India</t>
+  </si>
+  <si>
+    <t>Indonesia</t>
+  </si>
+  <si>
+    <t>Iran, Islamic Republic of</t>
+  </si>
+  <si>
+    <t>Iraq</t>
+  </si>
+  <si>
+    <t>Ireland</t>
+  </si>
+  <si>
+    <t>Isle of Man</t>
+  </si>
+  <si>
+    <t>Israel</t>
+  </si>
+  <si>
+    <t>Italy</t>
+  </si>
+  <si>
+    <t>Jamaica</t>
+  </si>
+  <si>
+    <t>Japan</t>
+  </si>
+  <si>
+    <t>Jersey</t>
+  </si>
+  <si>
+    <t>Jordan</t>
+  </si>
+  <si>
+    <t>Kazakhstan</t>
+  </si>
+  <si>
+    <t>Kenya</t>
+  </si>
+  <si>
+    <t>Kiribati</t>
+  </si>
+  <si>
+    <t>Korea, Democratic People's Republic of</t>
+  </si>
+  <si>
+    <t>Korea, Republic of</t>
+  </si>
+  <si>
+    <t>Kosovo</t>
+  </si>
+  <si>
+    <t>Kuwait</t>
+  </si>
+  <si>
+    <t>Kyrgyzstan</t>
+  </si>
+  <si>
+    <t>Lao People's Democratic Republic</t>
+  </si>
+  <si>
+    <t>Latvia</t>
+  </si>
+  <si>
+    <t>Lebanon</t>
+  </si>
+  <si>
+    <t>Lesotho</t>
+  </si>
+  <si>
+    <t>Liberia</t>
+  </si>
+  <si>
+    <t>Libyan Arab Jamahiriya</t>
+  </si>
+  <si>
+    <t>Liechtenstein</t>
+  </si>
+  <si>
+    <t>Lithuania</t>
+  </si>
+  <si>
+    <t>Luxembourg</t>
+  </si>
+  <si>
+    <t>Macao</t>
+  </si>
+  <si>
+    <t>Macedonia, the Former Yugoslav Republic of</t>
+  </si>
+  <si>
+    <t>Madagascar</t>
+  </si>
+  <si>
+    <t>Malawi</t>
+  </si>
+  <si>
+    <t>Malaysia</t>
+  </si>
+  <si>
+    <t>Maldives</t>
+  </si>
+  <si>
+    <t>Mali</t>
+  </si>
+  <si>
+    <t>Malta</t>
+  </si>
+  <si>
+    <t>Marshall Islands</t>
+  </si>
+  <si>
+    <t>Martinique</t>
+  </si>
+  <si>
+    <t>Mauritania</t>
+  </si>
+  <si>
+    <t>Mauritius</t>
+  </si>
+  <si>
+    <t>Mayotte</t>
+  </si>
+  <si>
+    <t>Mexico</t>
+  </si>
+  <si>
+    <t>Micronesia, Federated States of</t>
+  </si>
+  <si>
+    <t>Moldova, Republic of</t>
+  </si>
+  <si>
+    <t>Monaco</t>
+  </si>
+  <si>
+    <t>Mongolia</t>
+  </si>
+  <si>
+    <t>Montenegro</t>
+  </si>
+  <si>
+    <t>Montserrat</t>
+  </si>
+  <si>
+    <t>Morocco</t>
+  </si>
+  <si>
+    <t>Mozambique</t>
+  </si>
+  <si>
+    <t>Myanmar</t>
+  </si>
+  <si>
+    <t>Namibia</t>
+  </si>
+  <si>
+    <t>Nauru</t>
+  </si>
+  <si>
+    <t>Nepal</t>
+  </si>
+  <si>
+    <t>Netherlands</t>
+  </si>
+  <si>
+    <t>Netherlands Antilles</t>
+  </si>
+  <si>
+    <t>New Caledonia</t>
+  </si>
+  <si>
+    <t>New Zealand</t>
+  </si>
+  <si>
+    <t>Nicaragua</t>
+  </si>
+  <si>
+    <t>Niger</t>
+  </si>
+  <si>
+    <t>Nigeria</t>
+  </si>
+  <si>
+    <t>Niue</t>
+  </si>
+  <si>
+    <t>Norfolk Island</t>
+  </si>
+  <si>
+    <t>Northern Mariana Islands</t>
+  </si>
+  <si>
+    <t>Norway</t>
+  </si>
+  <si>
+    <t>Oman</t>
+  </si>
+  <si>
+    <t>Pakistan</t>
+  </si>
+  <si>
+    <t>Palau</t>
+  </si>
+  <si>
+    <t>Palestinian Territory, Occupied</t>
+  </si>
+  <si>
+    <t>Panama</t>
+  </si>
+  <si>
+    <t>Papua New Guinea</t>
+  </si>
+  <si>
+    <t>Paraguay</t>
+  </si>
+  <si>
+    <t>Peru</t>
+  </si>
+  <si>
+    <t>Philippines</t>
+  </si>
+  <si>
+    <t>Pitcairn</t>
+  </si>
+  <si>
+    <t>Poland</t>
+  </si>
+  <si>
+    <t>Portugal</t>
+  </si>
+  <si>
+    <t>Puerto Rico</t>
+  </si>
+  <si>
+    <t>Qatar</t>
+  </si>
+  <si>
+    <t>Reunion</t>
+  </si>
+  <si>
+    <t>Romania</t>
+  </si>
+  <si>
+    <t>Russian Federation</t>
+  </si>
+  <si>
+    <t>Rwanda</t>
+  </si>
+  <si>
+    <t>Saint Barthelemy</t>
+  </si>
+  <si>
+    <t>Saint Helena</t>
+  </si>
+  <si>
+    <t>Saint Kitts and Nevis</t>
+  </si>
+  <si>
+    <t>Saint Lucia</t>
+  </si>
+  <si>
+    <t>Saint Martin</t>
+  </si>
+  <si>
+    <t>Saint Pierre and Miquelon</t>
+  </si>
+  <si>
+    <t>Saint Vincent and the Grenadines</t>
+  </si>
+  <si>
+    <t>Samoa</t>
+  </si>
+  <si>
+    <t>San Marino</t>
+  </si>
+  <si>
+    <t>Sao Tome and Principe</t>
+  </si>
+  <si>
+    <t>Saudi Arabia</t>
+  </si>
+  <si>
+    <t>Senegal</t>
+  </si>
+  <si>
+    <t>Serbia</t>
+  </si>
+  <si>
+    <t>Serbia and Montenegro</t>
+  </si>
+  <si>
+    <t>Seychelles</t>
+  </si>
+  <si>
+    <t>Sierra Leone</t>
+  </si>
+  <si>
+    <t>Singapore</t>
+  </si>
+  <si>
+    <t>Sint Maarten</t>
+  </si>
+  <si>
+    <t>Slovakia</t>
+  </si>
+  <si>
+    <t>Slovenia</t>
+  </si>
+  <si>
+    <t>Solomon Islands</t>
+  </si>
+  <si>
+    <t>Somalia</t>
+  </si>
+  <si>
+    <t>South Africa</t>
+  </si>
+  <si>
+    <t>South Georgia and the South Sandwich Islands</t>
+  </si>
+  <si>
+    <t>South Sudan</t>
+  </si>
+  <si>
+    <t>Spain</t>
+  </si>
+  <si>
+    <t>Sri Lanka</t>
+  </si>
+  <si>
+    <t>Sudan</t>
+  </si>
+  <si>
+    <t>Suriname</t>
+  </si>
+  <si>
+    <t>Svalbard and Jan Mayen</t>
+  </si>
+  <si>
+    <t>Swaziland</t>
+  </si>
+  <si>
+    <t>Sweden</t>
+  </si>
+  <si>
+    <t>Switzerland</t>
+  </si>
+  <si>
+    <t>Syrian Arab Republic</t>
+  </si>
+  <si>
+    <t>Tajikistan</t>
+  </si>
+  <si>
+    <t>Thailand</t>
+  </si>
+  <si>
+    <t>Timor-Leste</t>
+  </si>
+  <si>
+    <t>Togo</t>
+  </si>
+  <si>
+    <t>Tokelau</t>
+  </si>
+  <si>
+    <t>Tonga</t>
+  </si>
+  <si>
+    <t>Trinidad and Tobago</t>
+  </si>
+  <si>
+    <t>Tunisia</t>
+  </si>
+  <si>
+    <t>Turkey</t>
+  </si>
+  <si>
+    <t>Turkmenistan</t>
+  </si>
+  <si>
+    <t>Turks and Caicos Islands</t>
+  </si>
+  <si>
+    <t>Tuvalu</t>
+  </si>
+  <si>
+    <t>Uganda</t>
+  </si>
+  <si>
+    <t>Ukraine</t>
+  </si>
+  <si>
+    <t>United Arab Emirates</t>
+  </si>
+  <si>
+    <t>United Kingdom</t>
+  </si>
+  <si>
+    <t>United States</t>
+  </si>
+  <si>
+    <t>United States Minor Outlying Islands</t>
+  </si>
+  <si>
+    <t>Uruguay</t>
+  </si>
+  <si>
+    <t>Uzbekistan</t>
+  </si>
+  <si>
+    <t>Vanuatu</t>
+  </si>
+  <si>
+    <t>Venezuela</t>
+  </si>
+  <si>
+    <t>Viet Nam</t>
+  </si>
+  <si>
+    <t>Virgin Islands, British</t>
+  </si>
+  <si>
+    <t>Virgin Islands, U.s.</t>
+  </si>
+  <si>
+    <t>Wallis and Futuna</t>
+  </si>
+  <si>
+    <t>Western Sahara</t>
+  </si>
+  <si>
+    <t>Yemen</t>
+  </si>
+  <si>
+    <t>Zambia</t>
+  </si>
+  <si>
+    <t>Zimbabwe</t>
+  </si>
+  <si>
+    <t>Taiwan</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Tanzania</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Location
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="微軟正黑體"/>
+        <family val="2"/>
+        <charset val="136"/>
+      </rPr>
+      <t>所處國別</t>
+    </r>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
     <t>王小明</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -1320,40 +2096,35 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
+    <t>Manager</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Engineering </t>
+  </si>
+  <si>
+    <t>ACER</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>ymhsieh@mail.ntust.edu.tw</t>
+  </si>
+  <si>
+    <t>212f2f@gmail.com</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Taiwan</t>
+  </si>
+  <si>
     <t>Professor</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>ymhsieh@mail.ntust.edu.tw</t>
-  </si>
-  <si>
     <t>Department of Civil and Construction Engineering</t>
   </si>
   <si>
-    <t>Manager</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">Engineering </t>
-  </si>
-  <si>
-    <t>ACER</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>212f2f@gmail.com</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>adv</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>National Taiwan University of Science and Technology</t>
-  </si>
-  <si>
-    <t>Taiwan</t>
-    <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -2093,7 +2864,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -2130,23 +2901,20 @@
     <xf numFmtId="49" fontId="19" fillId="34" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="36" fillId="0" borderId="0" xfId="42" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="36" fillId="0" borderId="0" xfId="42" applyNumberFormat="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="43">
@@ -2487,32 +3255,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="18.75" customHeight="1">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
-      <c r="F1" s="16"/>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
     </row>
     <row r="2" spans="1:6" ht="409.5" customHeight="1">
-      <c r="A2" s="17" t="s">
+      <c r="A2" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="17"/>
-      <c r="C2" s="17"/>
-      <c r="D2" s="17"/>
-      <c r="E2" s="17"/>
-      <c r="F2" s="17"/>
+      <c r="B2" s="14"/>
+      <c r="C2" s="14"/>
+      <c r="D2" s="14"/>
+      <c r="E2" s="14"/>
+      <c r="F2" s="14"/>
     </row>
     <row r="9" spans="1:6" ht="32.25" customHeight="1">
-      <c r="A9" s="15"/>
-      <c r="B9" s="15"/>
-      <c r="C9" s="15"/>
-      <c r="D9" s="15"/>
-      <c r="E9" s="15"/>
-      <c r="F9" s="15"/>
+      <c r="A9" s="12"/>
+      <c r="B9" s="12"/>
+      <c r="C9" s="12"/>
+      <c r="D9" s="12"/>
+      <c r="E9" s="12"/>
+      <c r="F9" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -2533,8 +3301,8 @@
   </sheetPr>
   <dimension ref="A1:J16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H30" sqref="H30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.6640625" defaultRowHeight="16"/>
@@ -2546,8 +3314,8 @@
     <col min="5" max="5" width="11.6640625" style="3" customWidth="1"/>
     <col min="6" max="6" width="17" style="3" customWidth="1"/>
     <col min="7" max="7" width="18.6640625" style="3" customWidth="1"/>
-    <col min="8" max="8" width="30.1640625" style="3" customWidth="1"/>
-    <col min="9" max="9" width="24.83203125" style="3" customWidth="1"/>
+    <col min="8" max="8" width="35" style="3" customWidth="1"/>
+    <col min="9" max="9" width="35.6640625" style="3" customWidth="1"/>
     <col min="10" max="10" width="31.1640625" style="3" customWidth="1"/>
     <col min="11" max="16384" width="9.6640625" style="3"/>
   </cols>
@@ -2583,63 +3351,71 @@
         <v>67</v>
       </c>
       <c r="I2" s="8" t="s">
+        <v>329</v>
+      </c>
+      <c r="J2" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="J2" s="14"/>
     </row>
     <row r="3" spans="1:10">
       <c r="A3" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="B3" s="12" t="s">
-        <v>78</v>
+        <v>330</v>
+      </c>
+      <c r="B3" s="15" t="s">
+        <v>331</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>79</v>
+        <v>332</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>80</v>
+        <v>333</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>81</v>
+        <v>334</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>82</v>
+        <v>341</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>84</v>
+        <v>342</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>90</v>
+        <v>343</v>
       </c>
       <c r="I3" s="3" t="s">
-        <v>83</v>
+        <v>340</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>338</v>
       </c>
     </row>
     <row r="4" spans="1:10">
       <c r="A4" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="B4" s="12" t="s">
-        <v>78</v>
+        <v>330</v>
+      </c>
+      <c r="B4" s="15" t="s">
+        <v>331</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>79</v>
+        <v>332</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>81</v>
+        <v>334</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>82</v>
+        <v>341</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>84</v>
+        <v>342</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>90</v>
+        <v>343</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>89</v>
+        <v>340</v>
+      </c>
+      <c r="J4" s="16" t="s">
+        <v>339</v>
       </c>
     </row>
     <row r="16" spans="1:10">
@@ -2648,10 +3424,23 @@
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="B3" r:id="rId1" xr:uid="{5BA8FB53-23C5-8348-AED5-2140A43388E6}"/>
-    <hyperlink ref="B4" r:id="rId2" xr:uid="{F249F3E7-831B-0345-BE9C-887C6BBF5023}"/>
+    <hyperlink ref="J4" r:id="rId1" xr:uid="{476313F9-8A7A-D648-ABE4-C6EF24D92A36}"/>
+    <hyperlink ref="B3" r:id="rId2" xr:uid="{21310C8A-4682-344E-80D5-E3276F62999D}"/>
+    <hyperlink ref="B4" r:id="rId3" xr:uid="{E01B6EC1-D407-4B4E-AB87-89B2D7AADA81}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{330ADD8D-6863-45B4-B3FB-B0CED901FF54}">
+          <x14:formula1>
+            <xm:f>工作表1!$A$3:$IR$3</xm:f>
+          </x14:formula1>
+          <xm:sqref>I3:I1048576</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -2662,8 +3451,8 @@
   </sheetPr>
   <dimension ref="A1:J16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J3" sqref="J3:J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.6640625" defaultRowHeight="16"/>
@@ -2676,7 +3465,7 @@
     <col min="6" max="6" width="17" style="3" customWidth="1"/>
     <col min="7" max="7" width="29.6640625" style="3" customWidth="1"/>
     <col min="8" max="8" width="30.1640625" style="3" customWidth="1"/>
-    <col min="9" max="9" width="13.83203125" style="3" customWidth="1"/>
+    <col min="9" max="9" width="30.83203125" style="3" customWidth="1"/>
     <col min="10" max="10" width="31.1640625" style="3" customWidth="1"/>
     <col min="11" max="16384" width="9.6640625" style="3"/>
   </cols>
@@ -2720,60 +3509,60 @@
     </row>
     <row r="3" spans="1:10">
       <c r="A3" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="B3" s="12" t="s">
-        <v>78</v>
+        <v>330</v>
+      </c>
+      <c r="B3" s="15" t="s">
+        <v>331</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>79</v>
+        <v>332</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>80</v>
+        <v>333</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>81</v>
+        <v>334</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>85</v>
+        <v>335</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>86</v>
+        <v>336</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>87</v>
+        <v>337</v>
       </c>
       <c r="I3" s="3" t="s">
-        <v>91</v>
+        <v>340</v>
       </c>
       <c r="J3" s="3" t="s">
-        <v>83</v>
+        <v>338</v>
       </c>
     </row>
     <row r="4" spans="1:10">
       <c r="A4" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="B4" s="12" t="s">
-        <v>78</v>
+        <v>330</v>
+      </c>
+      <c r="B4" s="15" t="s">
+        <v>331</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>80</v>
+        <v>333</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>85</v>
+        <v>335</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>86</v>
+        <v>336</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>87</v>
+        <v>337</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="J4" s="13" t="s">
-        <v>88</v>
+        <v>340</v>
+      </c>
+      <c r="J4" s="16" t="s">
+        <v>339</v>
       </c>
     </row>
     <row r="16" spans="1:10">
@@ -2782,19 +3571,25 @@
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="B3" r:id="rId1" xr:uid="{05BA278A-83D3-374B-8041-5B8CDB4C0FD9}"/>
-    <hyperlink ref="B4" r:id="rId2" xr:uid="{07C1EFAD-3584-8747-9A6C-C4454DD587D4}"/>
-    <hyperlink ref="J4" r:id="rId3" xr:uid="{C696DA48-7602-EF42-A161-01BFA274FE5D}"/>
+    <hyperlink ref="B3" r:id="rId1" xr:uid="{4B384F30-334D-1049-84F3-DF9226FE3689}"/>
+    <hyperlink ref="B4" r:id="rId2" xr:uid="{DD7B7C47-3F5B-B747-872D-C8C1834165D0}"/>
+    <hyperlink ref="J4" r:id="rId3" xr:uid="{73913C01-877D-814E-A7BF-36DE48A96D34}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{5337837A-E763-493C-8177-718A09A8971D}">
           <x14:formula1>
             <xm:f>工作表3!$A$2:$A$58</xm:f>
           </x14:formula1>
-          <xm:sqref>G3:G1048576</xm:sqref>
+          <xm:sqref>G5:G1048576</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{3AE16C18-18E0-49DB-A535-AAA19EB61937}">
+          <x14:formula1>
+            <xm:f>工作表1!$A$3:$IR$3</xm:f>
+          </x14:formula1>
+          <xm:sqref>I3:I1048576</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -2803,6 +3598,781 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F5AF902-A1E8-4FC6-A31D-C9CD744A2D1C}">
+  <dimension ref="A3:IR3"/>
+  <sheetViews>
+    <sheetView topLeftCell="HL1" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="3" spans="1:252">
+      <c r="A3" t="s">
+        <v>77</v>
+      </c>
+      <c r="B3" t="s">
+        <v>78</v>
+      </c>
+      <c r="C3" t="s">
+        <v>79</v>
+      </c>
+      <c r="D3" t="s">
+        <v>80</v>
+      </c>
+      <c r="E3" t="s">
+        <v>81</v>
+      </c>
+      <c r="F3" t="s">
+        <v>82</v>
+      </c>
+      <c r="G3" t="s">
+        <v>83</v>
+      </c>
+      <c r="H3" t="s">
+        <v>84</v>
+      </c>
+      <c r="I3" t="s">
+        <v>85</v>
+      </c>
+      <c r="J3" t="s">
+        <v>86</v>
+      </c>
+      <c r="K3" t="s">
+        <v>87</v>
+      </c>
+      <c r="L3" t="s">
+        <v>88</v>
+      </c>
+      <c r="M3" t="s">
+        <v>89</v>
+      </c>
+      <c r="N3" t="s">
+        <v>90</v>
+      </c>
+      <c r="O3" t="s">
+        <v>91</v>
+      </c>
+      <c r="P3" t="s">
+        <v>92</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>93</v>
+      </c>
+      <c r="R3" t="s">
+        <v>94</v>
+      </c>
+      <c r="S3" t="s">
+        <v>95</v>
+      </c>
+      <c r="T3" t="s">
+        <v>96</v>
+      </c>
+      <c r="U3" t="s">
+        <v>97</v>
+      </c>
+      <c r="V3" t="s">
+        <v>98</v>
+      </c>
+      <c r="W3" t="s">
+        <v>99</v>
+      </c>
+      <c r="X3" t="s">
+        <v>100</v>
+      </c>
+      <c r="Y3" t="s">
+        <v>101</v>
+      </c>
+      <c r="Z3" t="s">
+        <v>102</v>
+      </c>
+      <c r="AA3" t="s">
+        <v>103</v>
+      </c>
+      <c r="AB3" t="s">
+        <v>104</v>
+      </c>
+      <c r="AC3" t="s">
+        <v>105</v>
+      </c>
+      <c r="AD3" t="s">
+        <v>106</v>
+      </c>
+      <c r="AE3" t="s">
+        <v>107</v>
+      </c>
+      <c r="AF3" t="s">
+        <v>108</v>
+      </c>
+      <c r="AG3" t="s">
+        <v>109</v>
+      </c>
+      <c r="AH3" t="s">
+        <v>110</v>
+      </c>
+      <c r="AI3" t="s">
+        <v>111</v>
+      </c>
+      <c r="AJ3" t="s">
+        <v>112</v>
+      </c>
+      <c r="AK3" t="s">
+        <v>113</v>
+      </c>
+      <c r="AL3" t="s">
+        <v>114</v>
+      </c>
+      <c r="AM3" t="s">
+        <v>115</v>
+      </c>
+      <c r="AN3" t="s">
+        <v>116</v>
+      </c>
+      <c r="AO3" t="s">
+        <v>117</v>
+      </c>
+      <c r="AP3" t="s">
+        <v>118</v>
+      </c>
+      <c r="AQ3" t="s">
+        <v>119</v>
+      </c>
+      <c r="AR3" t="s">
+        <v>120</v>
+      </c>
+      <c r="AS3" t="s">
+        <v>121</v>
+      </c>
+      <c r="AT3" t="s">
+        <v>122</v>
+      </c>
+      <c r="AU3" t="s">
+        <v>123</v>
+      </c>
+      <c r="AV3" t="s">
+        <v>124</v>
+      </c>
+      <c r="AW3" t="s">
+        <v>125</v>
+      </c>
+      <c r="AX3" t="s">
+        <v>126</v>
+      </c>
+      <c r="AY3" t="s">
+        <v>127</v>
+      </c>
+      <c r="AZ3" t="s">
+        <v>128</v>
+      </c>
+      <c r="BA3" t="s">
+        <v>129</v>
+      </c>
+      <c r="BB3" t="s">
+        <v>130</v>
+      </c>
+      <c r="BC3" t="s">
+        <v>131</v>
+      </c>
+      <c r="BD3" t="s">
+        <v>132</v>
+      </c>
+      <c r="BE3" t="s">
+        <v>133</v>
+      </c>
+      <c r="BF3" t="s">
+        <v>134</v>
+      </c>
+      <c r="BG3" t="s">
+        <v>135</v>
+      </c>
+      <c r="BH3" t="s">
+        <v>136</v>
+      </c>
+      <c r="BI3" t="s">
+        <v>137</v>
+      </c>
+      <c r="BJ3" t="s">
+        <v>138</v>
+      </c>
+      <c r="BK3" t="s">
+        <v>139</v>
+      </c>
+      <c r="BL3" t="s">
+        <v>140</v>
+      </c>
+      <c r="BM3" t="s">
+        <v>141</v>
+      </c>
+      <c r="BN3" t="s">
+        <v>142</v>
+      </c>
+      <c r="BO3" t="s">
+        <v>143</v>
+      </c>
+      <c r="BP3" t="s">
+        <v>144</v>
+      </c>
+      <c r="BQ3" t="s">
+        <v>145</v>
+      </c>
+      <c r="BR3" t="s">
+        <v>146</v>
+      </c>
+      <c r="BS3" t="s">
+        <v>147</v>
+      </c>
+      <c r="BT3" t="s">
+        <v>148</v>
+      </c>
+      <c r="BU3" t="s">
+        <v>149</v>
+      </c>
+      <c r="BV3" t="s">
+        <v>150</v>
+      </c>
+      <c r="BW3" t="s">
+        <v>151</v>
+      </c>
+      <c r="BX3" t="s">
+        <v>152</v>
+      </c>
+      <c r="BY3" t="s">
+        <v>153</v>
+      </c>
+      <c r="BZ3" t="s">
+        <v>154</v>
+      </c>
+      <c r="CA3" t="s">
+        <v>155</v>
+      </c>
+      <c r="CB3" t="s">
+        <v>156</v>
+      </c>
+      <c r="CC3" t="s">
+        <v>157</v>
+      </c>
+      <c r="CD3" t="s">
+        <v>158</v>
+      </c>
+      <c r="CE3" t="s">
+        <v>159</v>
+      </c>
+      <c r="CF3" t="s">
+        <v>160</v>
+      </c>
+      <c r="CG3" t="s">
+        <v>161</v>
+      </c>
+      <c r="CH3" t="s">
+        <v>162</v>
+      </c>
+      <c r="CI3" t="s">
+        <v>163</v>
+      </c>
+      <c r="CJ3" t="s">
+        <v>164</v>
+      </c>
+      <c r="CK3" t="s">
+        <v>165</v>
+      </c>
+      <c r="CL3" t="s">
+        <v>166</v>
+      </c>
+      <c r="CM3" t="s">
+        <v>167</v>
+      </c>
+      <c r="CN3" t="s">
+        <v>168</v>
+      </c>
+      <c r="CO3" t="s">
+        <v>169</v>
+      </c>
+      <c r="CP3" t="s">
+        <v>170</v>
+      </c>
+      <c r="CQ3" t="s">
+        <v>171</v>
+      </c>
+      <c r="CR3" t="s">
+        <v>172</v>
+      </c>
+      <c r="CS3" t="s">
+        <v>173</v>
+      </c>
+      <c r="CT3" t="s">
+        <v>174</v>
+      </c>
+      <c r="CU3" t="s">
+        <v>175</v>
+      </c>
+      <c r="CV3" t="s">
+        <v>176</v>
+      </c>
+      <c r="CW3" t="s">
+        <v>177</v>
+      </c>
+      <c r="CX3" t="s">
+        <v>178</v>
+      </c>
+      <c r="CY3" t="s">
+        <v>179</v>
+      </c>
+      <c r="CZ3" t="s">
+        <v>180</v>
+      </c>
+      <c r="DA3" t="s">
+        <v>181</v>
+      </c>
+      <c r="DB3" t="s">
+        <v>182</v>
+      </c>
+      <c r="DC3" t="s">
+        <v>183</v>
+      </c>
+      <c r="DD3" t="s">
+        <v>184</v>
+      </c>
+      <c r="DE3" t="s">
+        <v>185</v>
+      </c>
+      <c r="DF3" t="s">
+        <v>186</v>
+      </c>
+      <c r="DG3" t="s">
+        <v>187</v>
+      </c>
+      <c r="DH3" t="s">
+        <v>188</v>
+      </c>
+      <c r="DI3" t="s">
+        <v>189</v>
+      </c>
+      <c r="DJ3" t="s">
+        <v>190</v>
+      </c>
+      <c r="DK3" t="s">
+        <v>191</v>
+      </c>
+      <c r="DL3" t="s">
+        <v>192</v>
+      </c>
+      <c r="DM3" t="s">
+        <v>193</v>
+      </c>
+      <c r="DN3" t="s">
+        <v>194</v>
+      </c>
+      <c r="DO3" t="s">
+        <v>195</v>
+      </c>
+      <c r="DP3" t="s">
+        <v>196</v>
+      </c>
+      <c r="DQ3" t="s">
+        <v>197</v>
+      </c>
+      <c r="DR3" t="s">
+        <v>198</v>
+      </c>
+      <c r="DS3" t="s">
+        <v>199</v>
+      </c>
+      <c r="DT3" t="s">
+        <v>200</v>
+      </c>
+      <c r="DU3" t="s">
+        <v>201</v>
+      </c>
+      <c r="DV3" t="s">
+        <v>202</v>
+      </c>
+      <c r="DW3" t="s">
+        <v>203</v>
+      </c>
+      <c r="DX3" t="s">
+        <v>204</v>
+      </c>
+      <c r="DY3" t="s">
+        <v>205</v>
+      </c>
+      <c r="DZ3" t="s">
+        <v>206</v>
+      </c>
+      <c r="EA3" t="s">
+        <v>207</v>
+      </c>
+      <c r="EB3" t="s">
+        <v>208</v>
+      </c>
+      <c r="EC3" t="s">
+        <v>209</v>
+      </c>
+      <c r="ED3" t="s">
+        <v>210</v>
+      </c>
+      <c r="EE3" t="s">
+        <v>211</v>
+      </c>
+      <c r="EF3" t="s">
+        <v>212</v>
+      </c>
+      <c r="EG3" t="s">
+        <v>213</v>
+      </c>
+      <c r="EH3" t="s">
+        <v>214</v>
+      </c>
+      <c r="EI3" t="s">
+        <v>215</v>
+      </c>
+      <c r="EJ3" t="s">
+        <v>216</v>
+      </c>
+      <c r="EK3" t="s">
+        <v>217</v>
+      </c>
+      <c r="EL3" t="s">
+        <v>218</v>
+      </c>
+      <c r="EM3" t="s">
+        <v>219</v>
+      </c>
+      <c r="EN3" t="s">
+        <v>220</v>
+      </c>
+      <c r="EO3" t="s">
+        <v>221</v>
+      </c>
+      <c r="EP3" t="s">
+        <v>222</v>
+      </c>
+      <c r="EQ3" t="s">
+        <v>223</v>
+      </c>
+      <c r="ER3" t="s">
+        <v>224</v>
+      </c>
+      <c r="ES3" t="s">
+        <v>225</v>
+      </c>
+      <c r="ET3" t="s">
+        <v>226</v>
+      </c>
+      <c r="EU3" t="s">
+        <v>227</v>
+      </c>
+      <c r="EV3" t="s">
+        <v>228</v>
+      </c>
+      <c r="EW3" t="s">
+        <v>229</v>
+      </c>
+      <c r="EX3" t="s">
+        <v>230</v>
+      </c>
+      <c r="EY3" t="s">
+        <v>231</v>
+      </c>
+      <c r="EZ3" t="s">
+        <v>232</v>
+      </c>
+      <c r="FA3" t="s">
+        <v>233</v>
+      </c>
+      <c r="FB3" t="s">
+        <v>234</v>
+      </c>
+      <c r="FC3" t="s">
+        <v>235</v>
+      </c>
+      <c r="FD3" t="s">
+        <v>236</v>
+      </c>
+      <c r="FE3" t="s">
+        <v>237</v>
+      </c>
+      <c r="FF3" t="s">
+        <v>238</v>
+      </c>
+      <c r="FG3" t="s">
+        <v>239</v>
+      </c>
+      <c r="FH3" t="s">
+        <v>240</v>
+      </c>
+      <c r="FI3" t="s">
+        <v>241</v>
+      </c>
+      <c r="FJ3" t="s">
+        <v>242</v>
+      </c>
+      <c r="FK3" t="s">
+        <v>243</v>
+      </c>
+      <c r="FL3" t="s">
+        <v>244</v>
+      </c>
+      <c r="FM3" t="s">
+        <v>245</v>
+      </c>
+      <c r="FN3" t="s">
+        <v>246</v>
+      </c>
+      <c r="FO3" t="s">
+        <v>247</v>
+      </c>
+      <c r="FP3" t="s">
+        <v>248</v>
+      </c>
+      <c r="FQ3" t="s">
+        <v>249</v>
+      </c>
+      <c r="FR3" t="s">
+        <v>250</v>
+      </c>
+      <c r="FS3" t="s">
+        <v>251</v>
+      </c>
+      <c r="FT3" t="s">
+        <v>252</v>
+      </c>
+      <c r="FU3" t="s">
+        <v>253</v>
+      </c>
+      <c r="FV3" t="s">
+        <v>254</v>
+      </c>
+      <c r="FW3" t="s">
+        <v>255</v>
+      </c>
+      <c r="FX3" t="s">
+        <v>256</v>
+      </c>
+      <c r="FY3" t="s">
+        <v>257</v>
+      </c>
+      <c r="FZ3" t="s">
+        <v>258</v>
+      </c>
+      <c r="GA3" t="s">
+        <v>259</v>
+      </c>
+      <c r="GB3" t="s">
+        <v>260</v>
+      </c>
+      <c r="GC3" t="s">
+        <v>261</v>
+      </c>
+      <c r="GD3" t="s">
+        <v>262</v>
+      </c>
+      <c r="GE3" t="s">
+        <v>263</v>
+      </c>
+      <c r="GF3" t="s">
+        <v>264</v>
+      </c>
+      <c r="GG3" t="s">
+        <v>265</v>
+      </c>
+      <c r="GH3" t="s">
+        <v>266</v>
+      </c>
+      <c r="GI3" t="s">
+        <v>267</v>
+      </c>
+      <c r="GJ3" t="s">
+        <v>268</v>
+      </c>
+      <c r="GK3" t="s">
+        <v>269</v>
+      </c>
+      <c r="GL3" t="s">
+        <v>270</v>
+      </c>
+      <c r="GM3" t="s">
+        <v>271</v>
+      </c>
+      <c r="GN3" t="s">
+        <v>272</v>
+      </c>
+      <c r="GO3" t="s">
+        <v>273</v>
+      </c>
+      <c r="GP3" t="s">
+        <v>274</v>
+      </c>
+      <c r="GQ3" t="s">
+        <v>275</v>
+      </c>
+      <c r="GR3" t="s">
+        <v>276</v>
+      </c>
+      <c r="GS3" t="s">
+        <v>277</v>
+      </c>
+      <c r="GT3" t="s">
+        <v>278</v>
+      </c>
+      <c r="GU3" t="s">
+        <v>279</v>
+      </c>
+      <c r="GV3" t="s">
+        <v>280</v>
+      </c>
+      <c r="GW3" t="s">
+        <v>281</v>
+      </c>
+      <c r="GX3" t="s">
+        <v>282</v>
+      </c>
+      <c r="GY3" t="s">
+        <v>283</v>
+      </c>
+      <c r="GZ3" t="s">
+        <v>284</v>
+      </c>
+      <c r="HA3" t="s">
+        <v>285</v>
+      </c>
+      <c r="HB3" t="s">
+        <v>286</v>
+      </c>
+      <c r="HC3" t="s">
+        <v>287</v>
+      </c>
+      <c r="HD3" t="s">
+        <v>288</v>
+      </c>
+      <c r="HE3" t="s">
+        <v>289</v>
+      </c>
+      <c r="HF3" t="s">
+        <v>290</v>
+      </c>
+      <c r="HG3" t="s">
+        <v>291</v>
+      </c>
+      <c r="HH3" t="s">
+        <v>292</v>
+      </c>
+      <c r="HI3" t="s">
+        <v>293</v>
+      </c>
+      <c r="HJ3" t="s">
+        <v>294</v>
+      </c>
+      <c r="HK3" t="s">
+        <v>295</v>
+      </c>
+      <c r="HL3" t="s">
+        <v>296</v>
+      </c>
+      <c r="HM3" t="s">
+        <v>327</v>
+      </c>
+      <c r="HN3" t="s">
+        <v>297</v>
+      </c>
+      <c r="HO3" t="s">
+        <v>328</v>
+      </c>
+      <c r="HP3" t="s">
+        <v>298</v>
+      </c>
+      <c r="HQ3" t="s">
+        <v>299</v>
+      </c>
+      <c r="HR3" t="s">
+        <v>300</v>
+      </c>
+      <c r="HS3" t="s">
+        <v>301</v>
+      </c>
+      <c r="HT3" t="s">
+        <v>302</v>
+      </c>
+      <c r="HU3" t="s">
+        <v>303</v>
+      </c>
+      <c r="HV3" t="s">
+        <v>304</v>
+      </c>
+      <c r="HW3" t="s">
+        <v>305</v>
+      </c>
+      <c r="HX3" t="s">
+        <v>306</v>
+      </c>
+      <c r="HY3" t="s">
+        <v>307</v>
+      </c>
+      <c r="HZ3" t="s">
+        <v>308</v>
+      </c>
+      <c r="IA3" t="s">
+        <v>309</v>
+      </c>
+      <c r="IB3" t="s">
+        <v>310</v>
+      </c>
+      <c r="IC3" t="s">
+        <v>311</v>
+      </c>
+      <c r="ID3" t="s">
+        <v>312</v>
+      </c>
+      <c r="IE3" t="s">
+        <v>313</v>
+      </c>
+      <c r="IF3" t="s">
+        <v>314</v>
+      </c>
+      <c r="IG3" t="s">
+        <v>315</v>
+      </c>
+      <c r="IH3" t="s">
+        <v>316</v>
+      </c>
+      <c r="II3" t="s">
+        <v>317</v>
+      </c>
+      <c r="IJ3" t="s">
+        <v>318</v>
+      </c>
+      <c r="IK3" t="s">
+        <v>319</v>
+      </c>
+      <c r="IL3" t="s">
+        <v>320</v>
+      </c>
+      <c r="IM3" t="s">
+        <v>321</v>
+      </c>
+      <c r="IN3" t="s">
+        <v>322</v>
+      </c>
+      <c r="IO3" t="s">
+        <v>323</v>
+      </c>
+      <c r="IP3" t="s">
+        <v>324</v>
+      </c>
+      <c r="IQ3" t="s">
+        <v>325</v>
+      </c>
+      <c r="IR3" t="s">
+        <v>326</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="18" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2522C696-34B4-42D7-8963-2BC5DDB7C06B}">
   <dimension ref="A1:A58"/>
   <sheetViews>

</xml_diff>